<commit_message>
chore: calibration and firmware
</commit_message>
<xml_diff>
--- a/docs/uv_calibration.xlsx
+++ b/docs/uv_calibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Luis\Freelance\Projects\uvIoT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA1F793-6028-46FC-BCAC-BEF97EAD71C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8277F0-0F9A-4316-B47C-1A6A659033A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{14F11370-0A06-414A-B478-6F8EACB6ECB4}"/>
   </bookViews>
@@ -35,9 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Nread</t>
+  </si>
+  <si>
+    <t>Vref(volts)</t>
+  </si>
+  <si>
+    <t>Vmultimeter(volts)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +62,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,13 +103,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -83,6 +132,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95F516F9-1FFC-4E82-93B8-F49343F46D17}" name="Tabla1" displayName="Tabla1" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{95F516F9-1FFC-4E82-93B8-F49343F46D17}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{60B2D5EE-BF05-4471-84D9-9ECBBCEF0877}" name="Vmultimeter(volts)"/>
+    <tableColumn id="2" xr3:uid="{C31C6372-FB9B-4C51-9148-073A6AF475AE}" name="Nread"/>
+    <tableColumn id="3" xr3:uid="{78A218B2-FE50-4A6D-A15A-FFECE77EEA2A}" name="Resolution"/>
+    <tableColumn id="4" xr3:uid="{27C3D642-3714-40FD-AC8B-3C2F56DCAB66}" name="Vref(volts)" dataDxfId="0">
+      <calculatedColumnFormula>Tabla1[[#This Row],[Vmultimeter(volts)]]*Tabla1[[#This Row],[Resolution]]/Tabla1[[#This Row],[Nread]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,51 +446,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3370659-CA73-405D-AA64-99313F7F762F}">
-  <dimension ref="B2:G4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.05</v>
+      </c>
       <c r="B2">
-        <v>1.21</v>
+        <v>292</v>
       </c>
       <c r="C2">
-        <v>0.38</v>
-      </c>
-      <c r="D2">
-        <v>336</v>
-      </c>
-      <c r="E2">
         <v>1023</v>
       </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <f>F2/E2*D2</f>
-        <v>0.98533724340175954</v>
+      <c r="D2" s="2">
+        <f>Tabla1[[#This Row],[Vmultimeter(volts)]]*Tabla1[[#This Row],[Resolution]]/Tabla1[[#This Row],[Nread]]</f>
+        <v>3.6785958904109592</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1.03</v>
-      </c>
-      <c r="C4">
-        <v>1067</v>
-      </c>
-      <c r="D4">
-        <v>4096</v>
-      </c>
-      <c r="E4">
-        <f>B4*D4/C4</f>
-        <v>3.9539643861293348</v>
-      </c>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>